<commit_message>
2020 els posponed covid19 public
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="194">
   <si>
     <t xml:space="preserve">Ocupantes podrán contender en</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t xml:space="preserve">C:30, CE:12.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elec 2020 pospuesta covid19</t>
   </si>
   <si>
     <t xml:space="preserve">18oct</t>
@@ -797,27 +800,27 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
-      <selection pane="bottomRight" activeCell="C103" activeCellId="0" sqref="C103"/>
+      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="AG44" activeCellId="0" sqref="AG44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.2857142857143"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="78.6989795918367"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,7 +3153,9 @@
       <c r="AM19" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AN19" s="12"/>
+      <c r="AN19" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
       <c r="AQ19" s="11"/>
@@ -3227,7 +3232,7 @@
         <v>46</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W20" s="11" t="s">
         <v>46</v>
@@ -3278,7 +3283,7 @@
         <v>46</v>
       </c>
       <c r="AM20" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AN20" s="12"/>
       <c r="AO20" s="11"/>
@@ -3302,7 +3307,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>58</v>
@@ -3347,7 +3352,7 @@
         <v>46</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>46</v>
@@ -3380,7 +3385,7 @@
         <v>54</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AD21" s="6" t="s">
         <v>46</v>
@@ -3411,7 +3416,7 @@
       </c>
       <c r="AM21" s="6"/>
       <c r="AN21" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
@@ -3670,7 +3675,7 @@
         <v>46</v>
       </c>
       <c r="AM23" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AN23" s="14"/>
       <c r="AO23" s="6"/>
@@ -3694,7 +3699,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>58</v>
@@ -3724,7 +3729,7 @@
         <v>46</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N24" s="11" t="s">
         <v>46</v>
@@ -3742,7 +3747,7 @@
         <v>46</v>
       </c>
       <c r="S24" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T24" s="11" t="s">
         <v>46</v>
@@ -3837,7 +3842,7 @@
         <v>46</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>46</v>
@@ -3846,7 +3851,7 @@
         <v>46</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L25" s="11" t="s">
         <v>46</v>
@@ -3855,7 +3860,7 @@
         <v>46</v>
       </c>
       <c r="N25" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O25" s="11" t="s">
         <v>46</v>
@@ -3864,16 +3869,16 @@
         <v>46</v>
       </c>
       <c r="Q25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T25" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S25" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T25" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="U25" s="11" t="s">
         <v>46</v>
@@ -3897,7 +3902,7 @@
         <v>46</v>
       </c>
       <c r="AB25" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AC25" s="11" t="s">
         <v>46</v>
@@ -3930,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="AM25" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AN25" s="12"/>
       <c r="AO25" s="11"/>
@@ -3967,7 +3972,7 @@
         <v>46</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>46</v>
@@ -3976,7 +3981,7 @@
         <v>46</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>46</v>
@@ -3985,7 +3990,7 @@
         <v>46</v>
       </c>
       <c r="N26" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O26" s="11" t="s">
         <v>46</v>
@@ -3994,16 +3999,16 @@
         <v>46</v>
       </c>
       <c r="Q26" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T26" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S26" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T26" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="U26" s="11" t="s">
         <v>46</v>
@@ -4027,7 +4032,7 @@
         <v>46</v>
       </c>
       <c r="AB26" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AC26" s="11" t="s">
         <v>46</v>
@@ -4060,7 +4065,7 @@
         <v>46</v>
       </c>
       <c r="AM26" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AN26" s="12"/>
       <c r="AO26" s="11"/>
@@ -4084,7 +4089,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
@@ -4227,7 +4232,7 @@
         <v>46</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>46</v>
@@ -4357,7 +4362,7 @@
         <v>46</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>46</v>
@@ -4474,7 +4479,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>58</v>
@@ -4710,7 +4715,7 @@
         <v>46</v>
       </c>
       <c r="AM31" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AN31" s="12"/>
       <c r="AO31" s="11"/>
@@ -4840,7 +4845,7 @@
         <v>46</v>
       </c>
       <c r="AM32" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AN32" s="12"/>
       <c r="AO32" s="11"/>
@@ -4864,7 +4869,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
@@ -5227,7 +5232,7 @@
         <v>46</v>
       </c>
       <c r="AL35" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AM35" s="6" t="n">
         <v>149</v>
@@ -5254,7 +5259,7 @@
         <v>11</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>58</v>
@@ -5269,7 +5274,7 @@
         <v>46</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>46</v>
@@ -5524,7 +5529,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>46</v>
@@ -5644,7 +5649,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>58</v>
@@ -5671,7 +5676,7 @@
         <v>46</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>46</v>
@@ -5707,7 +5712,7 @@
         <v>46</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Y39" s="6" t="s">
         <v>46</v>
@@ -5790,7 +5795,7 @@
         <v>46</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>46</v>
@@ -5799,7 +5804,7 @@
         <v>46</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>46</v>
@@ -5808,7 +5813,7 @@
         <v>46</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>46</v>
@@ -5817,7 +5822,7 @@
         <v>46</v>
       </c>
       <c r="R40" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S40" s="6" t="s">
         <v>46</v>
@@ -5826,7 +5831,7 @@
         <v>46</v>
       </c>
       <c r="U40" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="V40" s="6" t="s">
         <v>46</v>
@@ -5920,7 +5925,7 @@
         <v>46</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>46</v>
@@ -5929,7 +5934,7 @@
         <v>46</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M41" s="6" t="s">
         <v>46</v>
@@ -5938,7 +5943,7 @@
         <v>46</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>46</v>
@@ -5947,7 +5952,7 @@
         <v>46</v>
       </c>
       <c r="R41" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S41" s="6" t="s">
         <v>46</v>
@@ -5956,7 +5961,7 @@
         <v>46</v>
       </c>
       <c r="U41" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>46</v>
@@ -6010,7 +6015,7 @@
         <v>46</v>
       </c>
       <c r="AM41" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AN41" s="14"/>
       <c r="AO41" s="6"/>
@@ -6034,7 +6039,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>58</v>
@@ -6061,7 +6066,7 @@
         <v>46</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M42" s="11" t="s">
         <v>46</v>
@@ -6079,7 +6084,7 @@
         <v>46</v>
       </c>
       <c r="R42" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="S42" s="11" t="s">
         <v>46</v>
@@ -6180,35 +6185,35 @@
         <v>46</v>
       </c>
       <c r="I43" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O43" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R43" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="J43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L43" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="M43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O43" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="P43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="R43" s="11" t="s">
-        <v>122</v>
-      </c>
       <c r="S43" s="11" t="s">
         <v>46</v>
       </c>
@@ -6216,7 +6221,7 @@
         <v>46</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="V43" s="11" t="s">
         <v>46</v>
@@ -6298,7 +6303,7 @@
         <v>67</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F44" s="11" t="n">
         <v>1</v>
@@ -6319,7 +6324,7 @@
         <v>46</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M44" s="11" t="s">
         <v>46</v>
@@ -6337,7 +6342,7 @@
         <v>46</v>
       </c>
       <c r="R44" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="S44" s="11" t="s">
         <v>46</v>
@@ -6346,7 +6351,7 @@
         <v>46</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="V44" s="11" t="s">
         <v>46</v>
@@ -6402,7 +6407,9 @@
       <c r="AM44" s="11" t="n">
         <v>125</v>
       </c>
-      <c r="AN44" s="12"/>
+      <c r="AN44" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="AO44" s="11"/>
       <c r="AP44" s="11"/>
       <c r="AQ44" s="11"/>
@@ -6424,7 +6431,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>58</v>
@@ -6439,7 +6446,7 @@
         <v>46</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>46</v>
@@ -6454,7 +6461,7 @@
         <v>46</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>46</v>
@@ -6567,13 +6574,13 @@
         <v>46</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>46</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>46</v>
@@ -6582,7 +6589,7 @@
         <v>46</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N46" s="6" t="s">
         <v>46</v>
@@ -6697,13 +6704,13 @@
         <v>46</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>46</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>46</v>
@@ -6712,7 +6719,7 @@
         <v>46</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N47" s="6" t="s">
         <v>46</v>
@@ -6790,7 +6797,7 @@
         <v>46</v>
       </c>
       <c r="AM47" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AN47" s="14"/>
       <c r="AO47" s="6"/>
@@ -6814,7 +6821,7 @@
         <v>15</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>58</v>
@@ -6981,7 +6988,7 @@
         <v>46</v>
       </c>
       <c r="P49" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q49" s="11" t="s">
         <v>46</v>
@@ -6990,7 +6997,7 @@
         <v>46</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T49" s="11" t="s">
         <v>46</v>
@@ -7111,7 +7118,7 @@
         <v>46</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q50" s="11" t="s">
         <v>46</v>
@@ -7120,7 +7127,7 @@
         <v>46</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T50" s="11" t="s">
         <v>46</v>
@@ -7204,7 +7211,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>58</v>
@@ -7219,7 +7226,7 @@
         <v>46</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>46</v>
@@ -7237,7 +7244,7 @@
         <v>46</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O51" s="6" t="s">
         <v>46</v>
@@ -7255,7 +7262,7 @@
         <v>46</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U51" s="6" t="s">
         <v>46</v>
@@ -7267,7 +7274,7 @@
         <v>46</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Y51" s="6" t="s">
         <v>46</v>
@@ -7347,7 +7354,7 @@
         <v>46</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>46</v>
@@ -7356,17 +7363,17 @@
         <v>46</v>
       </c>
       <c r="K52" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N52" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="L52" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M52" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N52" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="O52" s="6" t="s">
         <v>46</v>
       </c>
@@ -7374,7 +7381,7 @@
         <v>46</v>
       </c>
       <c r="Q52" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R52" s="6" t="s">
         <v>46</v>
@@ -7383,7 +7390,7 @@
         <v>46</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U52" s="6" t="s">
         <v>46</v>
@@ -7395,7 +7402,7 @@
         <v>46</v>
       </c>
       <c r="X52" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Y52" s="6" t="s">
         <v>46</v>
@@ -7477,7 +7484,7 @@
         <v>46</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>46</v>
@@ -7486,17 +7493,17 @@
         <v>46</v>
       </c>
       <c r="K53" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N53" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="L53" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N53" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="O53" s="6" t="s">
         <v>46</v>
       </c>
@@ -7504,7 +7511,7 @@
         <v>46</v>
       </c>
       <c r="Q53" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R53" s="6" t="s">
         <v>46</v>
@@ -7513,7 +7520,7 @@
         <v>46</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U53" s="6" t="s">
         <v>46</v>
@@ -7525,7 +7532,7 @@
         <v>46</v>
       </c>
       <c r="X53" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Y53" s="6" t="s">
         <v>46</v>
@@ -7594,7 +7601,7 @@
         <v>17</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>58</v>
@@ -7606,7 +7613,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H54" s="11" t="s">
         <v>46</v>
@@ -7734,7 +7741,7 @@
         <v>3</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>46</v>
@@ -7743,7 +7750,7 @@
         <v>46</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K55" s="11" t="s">
         <v>46</v>
@@ -7864,7 +7871,7 @@
         <v>2</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>46</v>
@@ -7873,7 +7880,7 @@
         <v>46</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K56" s="11" t="s">
         <v>46</v>
@@ -7984,7 +7991,7 @@
         <v>18</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>58</v>
@@ -8374,7 +8381,7 @@
         <v>19</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>58</v>
@@ -8653,7 +8660,7 @@
         <v>46</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K62" s="11" t="s">
         <v>46</v>
@@ -8764,7 +8771,7 @@
         <v>20</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>58</v>
@@ -9037,7 +9044,7 @@
         <v>46</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>46</v>
@@ -9046,7 +9053,7 @@
         <v>46</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L65" s="6" t="s">
         <v>46</v>
@@ -9055,7 +9062,7 @@
         <v>46</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O65" s="6" t="s">
         <v>46</v>
@@ -9064,16 +9071,16 @@
         <v>46</v>
       </c>
       <c r="Q65" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R65" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S65" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T65" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="R65" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S65" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="T65" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="U65" s="6" t="s">
         <v>46</v>
@@ -9154,7 +9161,7 @@
         <v>21</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>58</v>
@@ -9178,7 +9185,7 @@
         <v>46</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L66" s="11" t="s">
         <v>46</v>
@@ -9196,7 +9203,7 @@
         <v>46</v>
       </c>
       <c r="Q66" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R66" s="11" t="s">
         <v>46</v>
@@ -9297,7 +9304,7 @@
         <v>46</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>46</v>
@@ -9306,17 +9313,17 @@
         <v>46</v>
       </c>
       <c r="K67" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L67" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M67" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N67" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L67" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M67" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N67" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O67" s="11" t="s">
         <v>46</v>
       </c>
@@ -9324,7 +9331,7 @@
         <v>46</v>
       </c>
       <c r="Q67" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R67" s="11" t="s">
         <v>46</v>
@@ -9333,7 +9340,7 @@
         <v>46</v>
       </c>
       <c r="T67" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U67" s="11" t="s">
         <v>46</v>
@@ -9427,7 +9434,7 @@
         <v>46</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I68" s="11" t="s">
         <v>46</v>
@@ -9436,17 +9443,17 @@
         <v>46</v>
       </c>
       <c r="K68" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L68" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M68" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N68" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L68" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M68" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N68" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O68" s="11" t="s">
         <v>46</v>
       </c>
@@ -9454,7 +9461,7 @@
         <v>46</v>
       </c>
       <c r="Q68" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R68" s="11" t="s">
         <v>46</v>
@@ -9463,7 +9470,7 @@
         <v>46</v>
       </c>
       <c r="T68" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U68" s="11" t="s">
         <v>46</v>
@@ -9520,7 +9527,7 @@
         <v>46</v>
       </c>
       <c r="AM68" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AN68" s="12"/>
       <c r="AO68" s="11"/>
@@ -9544,7 +9551,7 @@
         <v>22</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>58</v>
@@ -9934,7 +9941,7 @@
         <v>23</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D72" s="10" t="s">
         <v>58</v>
@@ -9961,7 +9968,7 @@
         <v>46</v>
       </c>
       <c r="L72" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M72" s="11" t="s">
         <v>46</v>
@@ -10080,7 +10087,7 @@
         <v>46</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J73" s="11" t="s">
         <v>46</v>
@@ -10089,7 +10096,7 @@
         <v>46</v>
       </c>
       <c r="L73" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M73" s="11" t="s">
         <v>46</v>
@@ -10098,7 +10105,7 @@
         <v>46</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P73" s="11" t="s">
         <v>46</v>
@@ -10167,7 +10174,7 @@
         <v>46</v>
       </c>
       <c r="AL73" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AM73" s="11" t="n">
         <v>57</v>
@@ -10210,7 +10217,7 @@
         <v>46</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J74" s="11" t="s">
         <v>46</v>
@@ -10219,7 +10226,7 @@
         <v>46</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M74" s="11" t="s">
         <v>46</v>
@@ -10228,7 +10235,7 @@
         <v>46</v>
       </c>
       <c r="O74" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P74" s="11" t="s">
         <v>46</v>
@@ -10324,7 +10331,7 @@
         <v>24</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>58</v>
@@ -10594,7 +10601,7 @@
         <v>2</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>46</v>
@@ -10621,7 +10628,7 @@
         <v>46</v>
       </c>
       <c r="P77" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q77" s="6" t="s">
         <v>46</v>
@@ -10693,7 +10700,7 @@
         <v>114</v>
       </c>
       <c r="AN77" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AO77" s="6"/>
       <c r="AP77" s="6"/>
@@ -10716,7 +10723,7 @@
         <v>25</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>58</v>
@@ -10740,7 +10747,7 @@
         <v>46</v>
       </c>
       <c r="K78" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L78" s="11" t="s">
         <v>46</v>
@@ -10758,7 +10765,7 @@
         <v>46</v>
       </c>
       <c r="Q78" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R78" s="11" t="s">
         <v>46</v>
@@ -10859,7 +10866,7 @@
         <v>46</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I79" s="11" t="s">
         <v>46</v>
@@ -10868,17 +10875,17 @@
         <v>46</v>
       </c>
       <c r="K79" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L79" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M79" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N79" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L79" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M79" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N79" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O79" s="11" t="s">
         <v>46</v>
       </c>
@@ -10886,7 +10893,7 @@
         <v>46</v>
       </c>
       <c r="Q79" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R79" s="11" t="s">
         <v>46</v>
@@ -10895,7 +10902,7 @@
         <v>46</v>
       </c>
       <c r="T79" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="U79" s="11" t="s">
         <v>46</v>
@@ -10989,7 +10996,7 @@
         <v>46</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>46</v>
@@ -10998,17 +11005,17 @@
         <v>46</v>
       </c>
       <c r="K80" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L80" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M80" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N80" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L80" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M80" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N80" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O80" s="11" t="s">
         <v>46</v>
       </c>
@@ -11016,7 +11023,7 @@
         <v>46</v>
       </c>
       <c r="Q80" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R80" s="11" t="s">
         <v>46</v>
@@ -11025,7 +11032,7 @@
         <v>46</v>
       </c>
       <c r="T80" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="U80" s="11" t="s">
         <v>46</v>
@@ -11106,7 +11113,7 @@
         <v>26</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>58</v>
@@ -11342,7 +11349,7 @@
         <v>46</v>
       </c>
       <c r="AM82" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AN82" s="14"/>
       <c r="AO82" s="6"/>
@@ -11370,7 +11377,7 @@
         <v>67</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F83" s="6" t="n">
         <v>2</v>
@@ -11472,10 +11479,10 @@
         <v>46</v>
       </c>
       <c r="AM83" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AN83" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AO83" s="6"/>
       <c r="AP83" s="6"/>
@@ -11498,7 +11505,7 @@
         <v>27</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>58</v>
@@ -11510,7 +11517,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H84" s="11" t="s">
         <v>46</v>
@@ -11528,7 +11535,7 @@
         <v>46</v>
       </c>
       <c r="M84" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N84" s="11" t="s">
         <v>65</v>
@@ -11546,7 +11553,7 @@
         <v>46</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T84" s="11" t="s">
         <v>46</v>
@@ -11638,7 +11645,7 @@
         <v>4</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H85" s="11" t="s">
         <v>46</v>
@@ -11647,7 +11654,7 @@
         <v>46</v>
       </c>
       <c r="J85" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K85" s="11" t="s">
         <v>46</v>
@@ -11656,7 +11663,7 @@
         <v>46</v>
       </c>
       <c r="M85" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N85" s="11" t="s">
         <v>46</v>
@@ -11665,7 +11672,7 @@
         <v>46</v>
       </c>
       <c r="P85" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q85" s="11" t="s">
         <v>46</v>
@@ -11674,7 +11681,7 @@
         <v>46</v>
       </c>
       <c r="S85" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T85" s="11" t="s">
         <v>46</v>
@@ -11683,7 +11690,7 @@
         <v>46</v>
       </c>
       <c r="V85" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W85" s="11" t="s">
         <v>46</v>
@@ -11768,7 +11775,7 @@
         <v>2</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>46</v>
@@ -11777,7 +11784,7 @@
         <v>46</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K86" s="11" t="s">
         <v>46</v>
@@ -11786,7 +11793,7 @@
         <v>46</v>
       </c>
       <c r="M86" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N86" s="11" t="s">
         <v>46</v>
@@ -11795,7 +11802,7 @@
         <v>46</v>
       </c>
       <c r="P86" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q86" s="11" t="s">
         <v>46</v>
@@ -11804,7 +11811,7 @@
         <v>46</v>
       </c>
       <c r="S86" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T86" s="11" t="s">
         <v>46</v>
@@ -11813,7 +11820,7 @@
         <v>46</v>
       </c>
       <c r="V86" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W86" s="11" t="s">
         <v>46</v>
@@ -11888,7 +11895,7 @@
         <v>28</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>58</v>
@@ -11912,7 +11919,7 @@
         <v>46</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L87" s="6" t="s">
         <v>46</v>
@@ -11930,7 +11937,7 @@
         <v>46</v>
       </c>
       <c r="Q87" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R87" s="6" t="s">
         <v>46</v>
@@ -12031,7 +12038,7 @@
         <v>46</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I88" s="6" t="s">
         <v>46</v>
@@ -12040,7 +12047,7 @@
         <v>46</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L88" s="6" t="s">
         <v>46</v>
@@ -12049,7 +12056,7 @@
         <v>46</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O88" s="6" t="s">
         <v>46</v>
@@ -12058,7 +12065,7 @@
         <v>46</v>
       </c>
       <c r="Q88" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R88" s="6" t="s">
         <v>46</v>
@@ -12067,7 +12074,7 @@
         <v>46</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U88" s="6" t="s">
         <v>46</v>
@@ -12121,7 +12128,7 @@
         <v>46</v>
       </c>
       <c r="AL88" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AM88" s="6" t="n">
         <v>25</v>
@@ -12161,7 +12168,7 @@
         <v>46</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I89" s="6" t="s">
         <v>46</v>
@@ -12170,7 +12177,7 @@
         <v>46</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L89" s="6" t="s">
         <v>46</v>
@@ -12179,7 +12186,7 @@
         <v>46</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O89" s="6" t="s">
         <v>46</v>
@@ -12188,7 +12195,7 @@
         <v>46</v>
       </c>
       <c r="Q89" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R89" s="6" t="s">
         <v>46</v>
@@ -12197,7 +12204,7 @@
         <v>46</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U89" s="6" t="s">
         <v>46</v>
@@ -12278,7 +12285,7 @@
         <v>29</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D90" s="10" t="s">
         <v>58</v>
@@ -12302,7 +12309,7 @@
         <v>46</v>
       </c>
       <c r="K90" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L90" s="11" t="s">
         <v>46</v>
@@ -12320,7 +12327,7 @@
         <v>46</v>
       </c>
       <c r="Q90" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R90" s="11" t="s">
         <v>46</v>
@@ -12421,7 +12428,7 @@
         <v>46</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I91" s="11" t="s">
         <v>46</v>
@@ -12430,17 +12437,17 @@
         <v>46</v>
       </c>
       <c r="K91" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L91" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M91" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N91" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L91" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M91" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N91" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O91" s="11" t="s">
         <v>46</v>
       </c>
@@ -12448,7 +12455,7 @@
         <v>46</v>
       </c>
       <c r="Q91" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R91" s="11" t="s">
         <v>46</v>
@@ -12457,7 +12464,7 @@
         <v>46</v>
       </c>
       <c r="T91" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U91" s="11" t="s">
         <v>46</v>
@@ -12548,7 +12555,7 @@
         <v>2</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H92" s="11" t="s">
         <v>46</v>
@@ -12560,17 +12567,17 @@
         <v>46</v>
       </c>
       <c r="K92" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L92" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M92" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N92" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L92" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M92" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N92" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="O92" s="11" t="s">
         <v>46</v>
       </c>
@@ -12578,7 +12585,7 @@
         <v>46</v>
       </c>
       <c r="Q92" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R92" s="11" t="s">
         <v>46</v>
@@ -12587,7 +12594,7 @@
         <v>46</v>
       </c>
       <c r="T92" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U92" s="11" t="s">
         <v>46</v>
@@ -12668,7 +12675,7 @@
         <v>30</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>58</v>
@@ -12826,7 +12833,7 @@
         <v>46</v>
       </c>
       <c r="M94" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N94" s="6" t="s">
         <v>46</v>
@@ -12847,7 +12854,7 @@
         <v>46</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U94" s="6" t="s">
         <v>46</v>
@@ -12932,13 +12939,13 @@
         <v>67</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F95" s="6" t="n">
         <v>1</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>46</v>
@@ -12947,7 +12954,7 @@
         <v>46</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K95" s="6" t="s">
         <v>46</v>
@@ -12956,7 +12963,7 @@
         <v>46</v>
       </c>
       <c r="M95" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N95" s="6" t="s">
         <v>46</v>
@@ -12977,7 +12984,7 @@
         <v>46</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U95" s="6" t="s">
         <v>46</v>
@@ -13031,7 +13038,7 @@
         <v>46</v>
       </c>
       <c r="AL95" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AM95" s="6" t="n">
         <v>70</v>
@@ -13058,7 +13065,7 @@
         <v>31</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>58</v>
@@ -13073,7 +13080,7 @@
         <v>46</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>46</v>
@@ -13091,7 +13098,7 @@
         <v>46</v>
       </c>
       <c r="N96" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O96" s="11" t="s">
         <v>46</v>
@@ -13109,7 +13116,7 @@
         <v>46</v>
       </c>
       <c r="T96" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="U96" s="11" t="s">
         <v>46</v>
@@ -13201,7 +13208,7 @@
         <v>46</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>46</v>
@@ -13210,35 +13217,35 @@
         <v>46</v>
       </c>
       <c r="K97" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="L97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N97" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="O97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q97" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="R97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T97" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="L97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N97" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="O97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q97" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="R97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T97" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="U97" s="11" t="s">
         <v>46</v>
       </c>
@@ -13246,7 +13253,7 @@
         <v>46</v>
       </c>
       <c r="W97" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X97" s="11" t="s">
         <v>46</v>
@@ -13331,7 +13338,7 @@
         <v>46</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>46</v>
@@ -13340,35 +13347,35 @@
         <v>46</v>
       </c>
       <c r="K98" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="L98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N98" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="O98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q98" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="R98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T98" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="L98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N98" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="O98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q98" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="R98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T98" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="U98" s="11" t="s">
         <v>46</v>
       </c>
@@ -13376,7 +13383,7 @@
         <v>46</v>
       </c>
       <c r="W98" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X98" s="11" t="s">
         <v>46</v>
@@ -13448,7 +13455,7 @@
         <v>32</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>58</v>
@@ -13850,7 +13857,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
@@ -13871,7 +13878,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
@@ -13911,15 +13918,18 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -13946,19 +13956,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13966,10 +13977,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13977,10 +13988,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13988,10 +13999,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13999,21 +14010,21 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020 els in coa hgo postponed du to covid19 public
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -286,13 +286,13 @@
     <t xml:space="preserve">5sep</t>
   </si>
   <si>
+    <t xml:space="preserve">18oct</t>
+  </si>
+  <si>
     <t xml:space="preserve">C:30, CE:12.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Elec 2020 pospuesta covid19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18oct</t>
+    <t xml:space="preserve">Elec 2020 pospuesta covid19 fecha por confirmar</t>
   </si>
   <si>
     <t xml:space="preserve">C:30, CE:14.4</t>
@@ -800,27 +800,28 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="W25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AG44" activeCellId="0" sqref="AG44"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="AN44" activeCellId="0" sqref="AN44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="78.6989795918367"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="77.7551020408163"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,7 +3134,7 @@
         <v>46</v>
       </c>
       <c r="AG19" s="11" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="AH19" s="11" t="s">
         <v>46</v>
@@ -3151,10 +3152,10 @@
         <v>46</v>
       </c>
       <c r="AM19" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AN19" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO19" s="11"/>
       <c r="AP19" s="11"/>
@@ -3232,7 +3233,7 @@
         <v>46</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W20" s="11" t="s">
         <v>46</v>
@@ -6387,7 +6388,7 @@
         <v>46</v>
       </c>
       <c r="AG44" s="11" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="AH44" s="11" t="s">
         <v>46</v>
@@ -6408,7 +6409,7 @@
         <v>125</v>
       </c>
       <c r="AN44" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO44" s="11"/>
       <c r="AP44" s="11"/>
@@ -11690,7 +11691,7 @@
         <v>46</v>
       </c>
       <c r="V85" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W85" s="11" t="s">
         <v>46</v>
@@ -11820,7 +11821,7 @@
         <v>46</v>
       </c>
       <c r="V86" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W86" s="11" t="s">
         <v>46</v>
@@ -13914,12 +13915,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AN44 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13951,14 +13952,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="AN44 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixes error in mic gob 2018 2024 pub
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -800,28 +800,28 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="W25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="AN44" activeCellId="0" sqref="AN44"/>
+      <selection pane="bottomRight" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.8775510204082"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="77.7551020408163"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="76.8112244897959"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7202,7 +7202,7 @@
       <c r="AW50" s="12"/>
       <c r="AX50" s="12"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <f aca="false">+A50+1</f>
         <v>49</v>
@@ -7296,7 +7296,7 @@
         <v>46</v>
       </c>
       <c r="AE51" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AF51" s="6" t="s">
         <v>46</v>
@@ -7314,7 +7314,7 @@
         <v>46</v>
       </c>
       <c r="AK51" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AL51" s="6" t="s">
         <v>46</v>
@@ -7332,7 +7332,7 @@
       <c r="AW51" s="14"/>
       <c r="AX51" s="14"/>
     </row>
-    <row r="52" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <f aca="false">+A51+1</f>
         <v>50</v>
@@ -13915,12 +13915,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AN44 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13952,14 +13952,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="AN44 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixes some pre-1980 dates
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -800,28 +800,27 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="A52" activeCellId="0" sqref="A52"/>
+      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AG2" activeCellId="0" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="76.8112244897959"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="75.1887755102041"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,7 +2221,7 @@
         <v>46</v>
       </c>
       <c r="AE12" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AF12" s="11" t="s">
         <v>46</v>
@@ -2240,7 +2239,7 @@
         <v>46</v>
       </c>
       <c r="AK12" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AL12" s="11" t="s">
         <v>46</v>
@@ -2628,7 +2627,7 @@
         <v>46</v>
       </c>
       <c r="AK15" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AL15" s="6" t="s">
         <v>46</v>
@@ -3410,7 +3409,7 @@
         <v>46</v>
       </c>
       <c r="AK21" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AL21" s="6" t="s">
         <v>46</v>
@@ -8466,7 +8465,7 @@
         <v>46</v>
       </c>
       <c r="AE60" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AF60" s="11" t="s">
         <v>46</v>
@@ -8475,7 +8474,7 @@
         <v>46</v>
       </c>
       <c r="AH60" s="11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="AI60" s="11" t="s">
         <v>46</v>
@@ -13159,7 +13158,7 @@
         <v>46</v>
       </c>
       <c r="AH96" s="11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="AI96" s="11" t="s">
         <v>46</v>
@@ -13920,7 +13919,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13957,9 +13956,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adds ver reform dropping mun term limits pub
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="195">
   <si>
     <t xml:space="preserve">Ocupantes podrán contender en</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t xml:space="preserve">2sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12mayo2020 reforma const para adoptar reeleccion consecutiva</t>
   </si>
   <si>
     <t xml:space="preserve">Yucatán</t>
@@ -800,27 +803,28 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E90" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG2" activeCellId="0" sqref="AG2"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+      <selection pane="bottomRight" activeCell="G95" activeCellId="0" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="75.1887755102041"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="74.2448979591837"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12925,7 +12929,7 @@
       <c r="AW94" s="14"/>
       <c r="AX94" s="14"/>
     </row>
-    <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <f aca="false">+A94+1</f>
         <v>93</v>
@@ -12938,11 +12942,11 @@
       <c r="D95" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E95" s="6" t="s">
-        <v>126</v>
+      <c r="E95" s="6" t="n">
+        <v>2024</v>
       </c>
       <c r="F95" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>128</v>
@@ -13035,15 +13039,17 @@
         <v>46</v>
       </c>
       <c r="AK95" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AL95" s="6" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="AM95" s="6" t="n">
         <v>70</v>
       </c>
-      <c r="AN95" s="14"/>
+      <c r="AN95" s="14" t="s">
+        <v>169</v>
+      </c>
       <c r="AO95" s="6"/>
       <c r="AP95" s="6"/>
       <c r="AQ95" s="6"/>
@@ -13065,7 +13071,7 @@
         <v>31</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>58</v>
@@ -13098,7 +13104,7 @@
         <v>46</v>
       </c>
       <c r="N96" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O96" s="11" t="s">
         <v>46</v>
@@ -13116,7 +13122,7 @@
         <v>46</v>
       </c>
       <c r="T96" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="U96" s="11" t="s">
         <v>46</v>
@@ -13217,35 +13223,35 @@
         <v>46</v>
       </c>
       <c r="K97" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N97" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="O97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q97" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="R97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T97" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="L97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N97" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="O97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q97" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="R97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S97" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T97" s="11" t="s">
-        <v>171</v>
-      </c>
       <c r="U97" s="11" t="s">
         <v>46</v>
       </c>
@@ -13253,7 +13259,7 @@
         <v>46</v>
       </c>
       <c r="W97" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X97" s="11" t="s">
         <v>46</v>
@@ -13347,35 +13353,35 @@
         <v>46</v>
       </c>
       <c r="K98" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N98" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="O98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q98" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="R98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T98" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="L98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N98" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="O98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q98" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="R98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S98" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T98" s="11" t="s">
-        <v>171</v>
-      </c>
       <c r="U98" s="11" t="s">
         <v>46</v>
       </c>
@@ -13383,7 +13389,7 @@
         <v>46</v>
       </c>
       <c r="W98" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X98" s="11" t="s">
         <v>46</v>
@@ -13455,7 +13461,7 @@
         <v>32</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>58</v>
@@ -13857,7 +13863,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
@@ -13878,7 +13884,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
@@ -13919,17 +13925,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -13956,20 +13962,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13977,10 +13983,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13988,10 +13994,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13999,10 +14005,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14010,21 +14016,21 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chg sin 2021 go was coded in 2022
</commit_message>
<xml_diff>
--- a/fechasEleccionesMexicoDesde1994.xlsx
+++ b/fechasEleccionesMexicoDesde1994.xlsx
@@ -803,28 +803,26 @@
   <dimension ref="A1:AX104"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="S62" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK10" activeCellId="0" sqref="AK10:AK11"/>
+      <selection pane="bottomLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+      <selection pane="bottomRight" activeCell="AH78" activeCellId="0" sqref="AH78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="38" min="7" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.6632653061225"/>
     <col collapsed="false" hidden="false" max="48" min="40" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="73.4336734693878"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="236" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="72.6275510204082"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="235" min="51" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10820,10 +10818,10 @@
         <v>46</v>
       </c>
       <c r="AH78" s="11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="AI78" s="11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="AJ78" s="11" t="s">
         <v>46</v>
@@ -13920,13 +13918,10 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AK10:AK11 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -13957,14 +13952,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="AK10:AK11 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="44.2755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>